<commit_message>
Update datetime formatting for date established.
</commit_message>
<xml_diff>
--- a/_reference_data/wikipedia_date_established.xlsx
+++ b/_reference_data/wikipedia_date_established.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -358,7 +362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C62"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -367,930 +371,625 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>park_name</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>park_name</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>date_established</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Acadia</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>February 26, 1919</t>
-        </is>
+      <c r="B2" s="2" t="n">
+        <v>6997</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>American Samoa</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>October 31, 1988</t>
-        </is>
+      <c r="B3" s="2" t="n">
+        <v>32447</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>Arches</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>November 12, 1971</t>
-        </is>
+      <c r="B4" s="2" t="n">
+        <v>26249</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>Badlands</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>November 10, 1978</t>
-        </is>
+      <c r="B5" s="2" t="n">
+        <v>28804</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>Big Bend</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>June 12, 1944</t>
-        </is>
+      <c r="B6" s="2" t="n">
+        <v>16235</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>Biscayne</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>June 28, 1980</t>
-        </is>
+      <c r="B7" s="2" t="n">
+        <v>29400</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Black Canyon of the Gunnison</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>October 21, 1999</t>
-        </is>
+      <c r="B8" s="2" t="n">
+        <v>36454</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>Bryce Canyon</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>February 25, 1928</t>
-        </is>
+      <c r="B9" s="2" t="n">
+        <v>10283</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>Canyonlands</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>September 12, 1964</t>
-        </is>
+      <c r="B10" s="2" t="n">
+        <v>23632</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>Capitol Reef</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>December 18, 1971</t>
-        </is>
+      <c r="B11" s="2" t="n">
+        <v>26285</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>Carlsbad Caverns</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>May 14, 1930</t>
-        </is>
+      <c r="B12" s="2" t="n">
+        <v>11092</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>Channel Islands</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>March 5, 1980</t>
-        </is>
+      <c r="B13" s="2" t="n">
+        <v>29285</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>Congaree</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>November 10, 2003</t>
-        </is>
+      <c r="B14" s="2" t="n">
+        <v>37935</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>Crater Lake</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>May 22, 1902</t>
-        </is>
+      <c r="B15" s="2" t="n">
+        <v>873</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>Cuyahoga Valley</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>October 11, 2000</t>
-        </is>
+      <c r="B16" s="2" t="n">
+        <v>36810</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="B17" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Death Valley</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>October 31, 1994</t>
-        </is>
+      <c r="B17" s="2" t="n">
+        <v>34638</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="B18" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>Denali</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>February 26, 1917</t>
-        </is>
+      <c r="B18" s="2" t="n">
+        <v>6267</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B19" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Dry Tortugas</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>October 26, 1992</t>
-        </is>
+      <c r="B19" s="2" t="n">
+        <v>33903</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Everglades</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>May 30, 1934</t>
-        </is>
+      <c r="B20" s="2" t="n">
+        <v>12569</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>Gates of the Arctic</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>December 2, 1980</t>
-        </is>
+      <c r="B21" s="2" t="n">
+        <v>29557</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>Gateway Arch</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>February 22, 2018</t>
-        </is>
+      <c r="B22" s="2" t="n">
+        <v>43153</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>Glacier</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>May 11, 1910</t>
-        </is>
+      <c r="B23" s="2" t="n">
+        <v>3784</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Glacier Bay</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>December 2, 1980</t>
-        </is>
+      <c r="B24" s="2" t="n">
+        <v>29557</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>Grand Canyon</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>February 26, 1919</t>
-        </is>
+      <c r="B25" s="2" t="n">
+        <v>6997</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>Grand Teton</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>February 26, 1929</t>
-        </is>
+      <c r="B26" s="2" t="n">
+        <v>10650</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>Great Basin</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>October 27, 1986</t>
-        </is>
+      <c r="B27" s="2" t="n">
+        <v>31712</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>Great Sand Dunes</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>September 13, 2004</t>
-        </is>
+      <c r="B28" s="2" t="n">
+        <v>38243</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>Great Smoky Mountains</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>June 15, 1934</t>
-        </is>
+      <c r="B29" s="2" t="n">
+        <v>12585</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="inlineStr">
+      <c r="A30" t="inlineStr">
         <is>
           <t>Guadalupe Mountains</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>October 15, 1966</t>
-        </is>
+      <c r="B30" s="2" t="n">
+        <v>24395</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
+      <c r="A31" t="inlineStr">
         <is>
           <t>Haleakalā</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>August 1, 1916</t>
-        </is>
+      <c r="B31" s="2" t="n">
+        <v>6058</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="inlineStr">
+      <c r="A32" t="inlineStr">
         <is>
           <t>Hawaiʻi Volcanoes</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>August 1, 1916</t>
-        </is>
+      <c r="B32" s="2" t="n">
+        <v>6058</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="inlineStr">
+      <c r="A33" t="inlineStr">
         <is>
           <t>Hot Springs</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>March 4, 1921</t>
-        </is>
+      <c r="B33" s="2" t="n">
+        <v>7734</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="inlineStr">
+      <c r="A34" t="inlineStr">
         <is>
           <t>Indiana Dunes</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>February 15, 2019</t>
-        </is>
+      <c r="B34" s="2" t="n">
+        <v>43511</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="inlineStr">
+      <c r="A35" t="inlineStr">
         <is>
           <t>Isle Royale</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>April 3, 1940</t>
-        </is>
+      <c r="B35" s="2" t="n">
+        <v>14704</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="inlineStr">
+      <c r="A36" t="inlineStr">
         <is>
           <t>Joshua Tree</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>October 31, 1994</t>
-        </is>
+      <c r="B36" s="2" t="n">
+        <v>34638</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="inlineStr">
+      <c r="A37" t="inlineStr">
         <is>
           <t>Katmai</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>December 2, 1980</t>
-        </is>
+      <c r="B37" s="2" t="n">
+        <v>29557</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="inlineStr">
+      <c r="A38" t="inlineStr">
         <is>
           <t>Kenai Fjords</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>December 2, 1980</t>
-        </is>
+      <c r="B38" s="2" t="n">
+        <v>29557</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="inlineStr">
+      <c r="A39" t="inlineStr">
         <is>
           <t>Kings Canyon</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>March 4, 1940</t>
-        </is>
+      <c r="B39" s="2" t="n">
+        <v>14674</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="inlineStr">
+      <c r="A40" t="inlineStr">
         <is>
           <t>Kobuk Valley</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>December 2, 1980</t>
-        </is>
+      <c r="B40" s="2" t="n">
+        <v>29557</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="inlineStr">
+      <c r="A41" t="inlineStr">
         <is>
           <t>Lake Clark</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>December 2, 1980</t>
-        </is>
+      <c r="B41" s="2" t="n">
+        <v>29557</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="inlineStr">
+      <c r="A42" t="inlineStr">
         <is>
           <t>Lassen Volcanic</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>August 9, 1916</t>
-        </is>
+      <c r="B42" s="2" t="n">
+        <v>6066</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="B43" t="inlineStr">
+      <c r="A43" t="inlineStr">
         <is>
           <t>Mammoth Cave</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>July 1, 1941</t>
-        </is>
+      <c r="B43" s="2" t="n">
+        <v>15158</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="B44" t="inlineStr">
+      <c r="A44" t="inlineStr">
         <is>
           <t>Mesa Verde</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>June 29, 1906</t>
-        </is>
+      <c r="B44" s="2" t="n">
+        <v>2372</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="B45" t="inlineStr">
+      <c r="A45" t="inlineStr">
         <is>
           <t>Mount Rainier</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>March 2, 1899</t>
-        </is>
+      <c r="B45" s="2" t="n">
+        <v>-304</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="B46" t="inlineStr">
+      <c r="A46" t="inlineStr">
         <is>
           <t>North Cascades</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>October 2, 1968</t>
-        </is>
+      <c r="B46" s="2" t="n">
+        <v>25113</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="B47" t="inlineStr">
+      <c r="A47" t="inlineStr">
         <is>
           <t>Olympic</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>June 29, 1938</t>
-        </is>
+      <c r="B47" s="2" t="n">
+        <v>14060</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="B48" t="inlineStr">
+      <c r="A48" t="inlineStr">
         <is>
           <t>Petrified Forest</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>December 9, 1962</t>
-        </is>
+      <c r="B48" s="2" t="n">
+        <v>22989</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="B49" t="inlineStr">
+      <c r="A49" t="inlineStr">
         <is>
           <t>Pinnacles</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>January 10, 2013</t>
-        </is>
+      <c r="B49" s="2" t="n">
+        <v>41284</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="B50" t="inlineStr">
+      <c r="A50" t="inlineStr">
         <is>
           <t>Redwood</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>October 2, 1968</t>
-        </is>
+      <c r="B50" s="2" t="n">
+        <v>25113</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="B51" t="inlineStr">
+      <c r="A51" t="inlineStr">
         <is>
           <t>Rocky Mountain</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>January 26, 1915</t>
-        </is>
+      <c r="B51" s="2" t="n">
+        <v>5505</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
+      <c r="A52" t="inlineStr">
         <is>
           <t>Saguaro</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>October 14, 1994</t>
-        </is>
+      <c r="B52" s="2" t="n">
+        <v>34621</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
+      <c r="A53" t="inlineStr">
         <is>
           <t>Sequoia</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>September 25, 1890</t>
-        </is>
+      <c r="B53" s="2" t="n">
+        <v>-3384</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
+      <c r="A54" t="inlineStr">
         <is>
           <t>Shenandoah</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>December 26, 1935</t>
-        </is>
+      <c r="B54" s="2" t="n">
+        <v>13144</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
+      <c r="A55" t="inlineStr">
         <is>
           <t>Theodore Roosevelt</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>November 10, 1978</t>
-        </is>
+      <c r="B55" s="2" t="n">
+        <v>28804</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
+      <c r="A56" t="inlineStr">
         <is>
           <t>Virgin Islands</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>August 2, 1956</t>
-        </is>
+      <c r="B56" s="2" t="n">
+        <v>20669</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
+      <c r="A57" t="inlineStr">
         <is>
           <t>Voyageurs</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>January 8, 1971</t>
-        </is>
+      <c r="B57" s="2" t="n">
+        <v>25941</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
+      <c r="A58" t="inlineStr">
         <is>
           <t>Wind Cave</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>January 9, 1903</t>
-        </is>
+      <c r="B58" s="2" t="n">
+        <v>1105</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="n">
-        <v>57</v>
-      </c>
-      <c r="B59" t="inlineStr">
+      <c r="A59" t="inlineStr">
         <is>
           <t>Wrangell–St. Elias</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>December 2, 1980</t>
-        </is>
+      <c r="B59" s="2" t="n">
+        <v>29557</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="B60" t="inlineStr">
+      <c r="A60" t="inlineStr">
         <is>
           <t>Yellowstone</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>March 1, 1872</t>
-        </is>
+      <c r="B60" s="2" t="n">
+        <v>-10166</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="n">
-        <v>59</v>
-      </c>
-      <c r="B61" t="inlineStr">
+      <c r="A61" t="inlineStr">
         <is>
           <t>Yosemite</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>October 1, 1890</t>
-        </is>
+      <c r="B61" s="2" t="n">
+        <v>-3378</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="B62" t="inlineStr">
+      <c r="A62" t="inlineStr">
         <is>
           <t>Zion</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>November 19, 1919</t>
-        </is>
+      <c r="B62" s="2" t="n">
+        <v>7263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>